<commit_message>
maj 12122025 plan passage de poutre data
</commit_message>
<xml_diff>
--- a/Remote/ug16/Données/04/dist_liens.xlsx
+++ b/Remote/ug16/Données/04/dist_liens.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\Commun\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Mickaël\Documents\GitHub\ductaironline\Remote\ug16\Données\04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2237ED13-DDA8-454B-BFB8-45A111A1FEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7283D0-E43F-4580-9015-D325683BDDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
+    <workbookView xWindow="5580" yWindow="4350" windowWidth="21600" windowHeight="11295" xr2:uid="{10E80606-BDFD-48EA-859F-8B282D217FD1}"/>
   </bookViews>
   <sheets>
     <sheet name="dist_liens" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">dist_liens!$C$1:$V$175</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">dist_liens!$C$1:$V$182</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3480" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="278">
   <si>
     <t>id</t>
   </si>
@@ -680,18 +680,6 @@
     <t>POU</t>
   </si>
   <si>
-    <t>TAN</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/POU/tang.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/POU/dep.jpg</t>
-  </si>
-  <si>
-    <t>FAC</t>
-  </si>
-  <si>
     <t>CAD</t>
   </si>
   <si>
@@ -702,9 +690,6 @@
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/SG/image004.jpg</t>
-  </si>
-  <si>
-    <t>https://ductair.github.io/ductaironline/Drawings/POU/dessus.jpg</t>
   </si>
   <si>
     <t>https://ductair.github.io/ductaironline/Drawings/AUTRES/nondispo.jpg</t>
@@ -837,6 +822,57 @@
   </si>
   <si>
     <t>AXE</t>
+  </si>
+  <si>
+    <t>C0</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CDEP</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>CT1</t>
+  </si>
+  <si>
+    <t>CT2</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Dessus/inconnudessuspou.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Dessus/tanghautdessus.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Dessus/tangbasdessus,jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Dessus/dessus.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Dessus/deport,jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Cote/inconnucotepou.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Cote/centrecotepou.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Cote/tanghautpou.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Cote/dep.jpg</t>
+  </si>
+  <si>
+    <t>https://ductair.github.io/ductaironline/Drawings/POU/Cote/tangbaspou.jpg</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1282,11 @@
   <sheetPr codeName="Feuil36">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CD177"/>
+  <dimension ref="A1:CD184"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C177" sqref="C177"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G173" sqref="G173:CD179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2085,10 +2121,10 @@
         <v>28</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="G4">
         <v>120</v>
@@ -2581,10 +2617,10 @@
         <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G6">
         <v>120</v>
@@ -3576,7 +3612,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G10">
         <v>120</v>
@@ -4069,10 +4105,10 @@
         <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F12" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G12">
         <v>120</v>
@@ -4565,10 +4601,10 @@
         <v>32</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F14" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G14">
         <v>120</v>
@@ -7045,10 +7081,10 @@
         <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="G24">
         <v>120</v>
@@ -7541,10 +7577,10 @@
         <v>31</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F26" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G26">
         <v>120</v>
@@ -9029,10 +9065,10 @@
         <v>33</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F32" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="G32">
         <v>120</v>
@@ -9525,10 +9561,10 @@
         <v>33</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F34" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G34">
         <v>120</v>
@@ -12005,10 +12041,10 @@
         <v>28</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F44" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="G44">
         <v>120</v>
@@ -12501,10 +12537,10 @@
         <v>28</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F46" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G46">
         <v>120</v>
@@ -13989,10 +14025,10 @@
         <v>32</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F52" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G52">
         <v>120</v>
@@ -14485,10 +14521,10 @@
         <v>32</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F54" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G54">
         <v>120</v>
@@ -15480,7 +15516,7 @@
         <v>29</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="G58">
         <v>120</v>
@@ -16965,10 +17001,10 @@
         <v>31</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F64" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G64">
         <v>120</v>
@@ -17461,10 +17497,10 @@
         <v>31</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F66" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G66">
         <v>120</v>
@@ -18949,10 +18985,10 @@
         <v>33</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F72" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="G72">
         <v>120</v>
@@ -19445,10 +19481,10 @@
         <v>33</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F74" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G74">
         <v>120</v>
@@ -21925,10 +21961,10 @@
         <v>28</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F84" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="G84">
         <v>120</v>
@@ -22421,10 +22457,10 @@
         <v>28</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F86" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G86">
         <v>120</v>
@@ -23909,10 +23945,10 @@
         <v>32</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="F92" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="G92">
         <v>120</v>
@@ -24405,10 +24441,10 @@
         <v>32</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F94" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G94">
         <v>120</v>
@@ -26885,10 +26921,10 @@
         <v>31</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F104" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="G104">
         <v>120</v>
@@ -27381,10 +27417,10 @@
         <v>31</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F106" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G106">
         <v>120</v>
@@ -28869,10 +28905,10 @@
         <v>33</v>
       </c>
       <c r="E112" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="F112" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G112">
         <v>120</v>
@@ -29365,10 +29401,10 @@
         <v>33</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F114" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G114">
         <v>120</v>
@@ -31343,12 +31379,12 @@
         <v>45931</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="3"/>
       <c r="F122" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G122">
         <v>20</v>
@@ -32086,13 +32122,13 @@
         <v>141</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E125" s="3" t="s">
         <v>143</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="G125">
         <v>240</v>
@@ -32830,13 +32866,13 @@
         <v>141</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E128" s="3" t="s">
         <v>143</v>
       </c>
       <c r="F128" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G128">
         <v>240</v>
@@ -34566,13 +34602,13 @@
         <v>158</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E135" s="3" t="s">
         <v>143</v>
       </c>
       <c r="F135" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="G135">
         <v>240</v>
@@ -35310,13 +35346,13 @@
         <v>158</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E138" s="3" t="s">
         <v>143</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G138">
         <v>240</v>
@@ -40748,7 +40784,7 @@
         <v>195</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="G160">
         <v>170</v>
@@ -41964,7 +42000,7 @@
         <v>206</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="F165" t="s">
         <v>207</v>
@@ -42209,10 +42245,10 @@
         <v>206</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="G166">
         <v>240</v>
@@ -42266,7 +42302,7 @@
         <v>41</v>
       </c>
       <c r="X166">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y166" s="5" t="s">
         <v>118</v>
@@ -42944,7 +42980,7 @@
         <v>168</v>
       </c>
       <c r="F169" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G169">
         <v>250</v>
@@ -43180,16 +43216,16 @@
         <v>167</v>
       </c>
       <c r="B170" s="5">
-        <v>45693</v>
+        <v>46002</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D170" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F170" t="s">
-        <v>214</v>
+      <c r="D170" s="2">
+        <v>0</v>
+      </c>
+      <c r="F170" s="8" t="s">
+        <v>268</v>
       </c>
       <c r="G170">
         <v>250</v>
@@ -43425,16 +43461,16 @@
         <v>168</v>
       </c>
       <c r="B171" s="5">
-        <v>45693</v>
+        <v>46002</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>212</v>
       </c>
       <c r="D171" t="s">
-        <v>195</v>
-      </c>
-      <c r="F171" t="s">
-        <v>215</v>
+        <v>47</v>
+      </c>
+      <c r="F171" s="8" t="s">
+        <v>271</v>
       </c>
       <c r="G171">
         <v>250</v>
@@ -43670,16 +43706,16 @@
         <v>169</v>
       </c>
       <c r="B172" s="5">
-        <v>45693</v>
+        <v>46002</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>212</v>
       </c>
       <c r="D172" t="s">
-        <v>216</v>
-      </c>
-      <c r="F172" t="s">
-        <v>221</v>
+        <v>264</v>
+      </c>
+      <c r="F172" s="8" t="s">
+        <v>269</v>
       </c>
       <c r="G172">
         <v>250</v>
@@ -43915,19 +43951,22 @@
         <v>170</v>
       </c>
       <c r="B173" s="5">
-        <v>45693</v>
+        <v>46002</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F173" t="s">
-        <v>222</v>
+        <v>212</v>
+      </c>
+      <c r="D173" t="s">
+        <v>265</v>
+      </c>
+      <c r="F173" s="8" t="s">
+        <v>270</v>
       </c>
       <c r="G173">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H173">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="I173" s="2" t="s">
         <v>28</v>
@@ -43935,41 +43974,41 @@
       <c r="J173" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="K173" s="2">
-        <v>0</v>
+      <c r="K173" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="L173" s="2">
         <v>0</v>
       </c>
-      <c r="M173" s="2">
-        <v>0</v>
+      <c r="M173" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="N173" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="O173" s="2">
-        <v>0</v>
-      </c>
-      <c r="P173" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q173" s="2">
-        <v>0</v>
-      </c>
-      <c r="R173" s="2">
-        <v>0</v>
-      </c>
-      <c r="S173" s="2">
-        <v>0</v>
-      </c>
-      <c r="T173" s="2">
-        <v>0</v>
-      </c>
-      <c r="U173" s="2">
-        <v>0</v>
-      </c>
-      <c r="V173" s="2">
-        <v>0</v>
+      <c r="O173" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P173" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q173">
+        <v>0</v>
+      </c>
+      <c r="R173">
+        <v>0</v>
+      </c>
+      <c r="S173" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T173" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U173" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V173" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W173" s="2" t="s">
         <v>41</v>
@@ -43984,10 +44023,10 @@
         <v>0</v>
       </c>
       <c r="AA173">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB173">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC173">
         <v>0</v>
@@ -44157,43 +44196,46 @@
         <v>171</v>
       </c>
       <c r="B174" s="5">
-        <v>45693</v>
-      </c>
-      <c r="C174" t="s">
-        <v>218</v>
-      </c>
-      <c r="F174" t="s">
-        <v>222</v>
+        <v>46002</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D174" t="s">
+        <v>195</v>
+      </c>
+      <c r="F174" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="G174">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H174">
-        <v>170</v>
-      </c>
-      <c r="I174">
-        <v>0</v>
-      </c>
-      <c r="J174">
-        <v>0</v>
-      </c>
-      <c r="K174">
-        <v>0</v>
-      </c>
-      <c r="L174">
-        <v>0</v>
-      </c>
-      <c r="M174">
-        <v>0</v>
-      </c>
-      <c r="N174">
-        <v>0</v>
-      </c>
-      <c r="O174">
-        <v>0</v>
-      </c>
-      <c r="P174">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="I174" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J174" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K174" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L174" s="2">
+        <v>0</v>
+      </c>
+      <c r="M174" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N174" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O174" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P174" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="Q174">
         <v>0</v>
@@ -44201,17 +44243,17 @@
       <c r="R174">
         <v>0</v>
       </c>
-      <c r="S174">
-        <v>0</v>
-      </c>
-      <c r="T174">
-        <v>0</v>
-      </c>
-      <c r="U174">
-        <v>0</v>
-      </c>
-      <c r="V174">
-        <v>0</v>
+      <c r="S174" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T174" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U174" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V174" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W174" s="2" t="s">
         <v>41</v>
@@ -44226,10 +44268,10 @@
         <v>0</v>
       </c>
       <c r="AA174">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB174">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC174">
         <v>0</v>
@@ -44399,43 +44441,46 @@
         <v>172</v>
       </c>
       <c r="B175" s="5">
-        <v>45693</v>
-      </c>
-      <c r="C175" t="s">
-        <v>219</v>
-      </c>
-      <c r="F175" t="s">
-        <v>222</v>
+        <v>46002</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D175" t="s">
+        <v>261</v>
+      </c>
+      <c r="F175" s="8" t="s">
+        <v>273</v>
       </c>
       <c r="G175">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="H175">
-        <v>170</v>
-      </c>
-      <c r="I175">
-        <v>0</v>
-      </c>
-      <c r="J175">
-        <v>0</v>
-      </c>
-      <c r="K175">
-        <v>0</v>
-      </c>
-      <c r="L175">
-        <v>0</v>
-      </c>
-      <c r="M175">
-        <v>0</v>
-      </c>
-      <c r="N175">
-        <v>0</v>
-      </c>
-      <c r="O175">
-        <v>0</v>
-      </c>
-      <c r="P175">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="I175" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J175" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K175" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L175" s="2">
+        <v>0</v>
+      </c>
+      <c r="M175" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N175" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O175" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P175" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="Q175">
         <v>0</v>
@@ -44443,17 +44488,17 @@
       <c r="R175">
         <v>0</v>
       </c>
-      <c r="S175">
-        <v>0</v>
-      </c>
-      <c r="T175">
-        <v>0</v>
-      </c>
-      <c r="U175">
-        <v>0</v>
-      </c>
-      <c r="V175">
-        <v>0</v>
+      <c r="S175" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T175" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U175" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V175" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W175" s="2" t="s">
         <v>41</v>
@@ -44468,10 +44513,10 @@
         <v>0</v>
       </c>
       <c r="AA175">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB175">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC175">
         <v>0</v>
@@ -44641,43 +44686,46 @@
         <v>173</v>
       </c>
       <c r="B176" s="5">
-        <v>45693</v>
-      </c>
-      <c r="C176">
-        <v>404</v>
+        <v>46002</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D176" t="s">
+        <v>262</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="G176">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="H176">
-        <v>180</v>
-      </c>
-      <c r="I176">
-        <v>0</v>
-      </c>
-      <c r="J176">
-        <v>0</v>
-      </c>
-      <c r="K176">
-        <v>0</v>
-      </c>
-      <c r="L176">
-        <v>0</v>
-      </c>
-      <c r="M176">
-        <v>0</v>
-      </c>
-      <c r="N176">
-        <v>0</v>
-      </c>
-      <c r="O176">
-        <v>0</v>
-      </c>
-      <c r="P176">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="I176" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J176" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K176" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L176" s="2">
+        <v>0</v>
+      </c>
+      <c r="M176" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N176" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O176" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P176" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="Q176">
         <v>0</v>
@@ -44685,17 +44733,17 @@
       <c r="R176">
         <v>0</v>
       </c>
-      <c r="S176">
-        <v>0</v>
-      </c>
-      <c r="T176">
-        <v>0</v>
-      </c>
-      <c r="U176">
-        <v>0</v>
-      </c>
-      <c r="V176">
-        <v>0</v>
+      <c r="S176" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T176" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U176" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V176" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W176" s="2" t="s">
         <v>41</v>
@@ -44710,10 +44758,10 @@
         <v>0</v>
       </c>
       <c r="AA176">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB176">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC176">
         <v>0</v>
@@ -44880,46 +44928,49 @@
     </row>
     <row r="177" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A177" s="4">
-        <v>404</v>
+        <v>174</v>
       </c>
       <c r="B177" s="5">
-        <v>45693</v>
-      </c>
-      <c r="C177">
-        <v>404</v>
+        <v>46002</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D177" t="s">
+        <v>266</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>262</v>
+        <v>275</v>
       </c>
       <c r="G177">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="H177">
-        <v>180</v>
-      </c>
-      <c r="I177">
-        <v>0</v>
-      </c>
-      <c r="J177">
-        <v>0</v>
-      </c>
-      <c r="K177">
-        <v>0</v>
-      </c>
-      <c r="L177">
-        <v>0</v>
-      </c>
-      <c r="M177">
-        <v>0</v>
-      </c>
-      <c r="N177">
-        <v>0</v>
-      </c>
-      <c r="O177">
-        <v>0</v>
-      </c>
-      <c r="P177">
-        <v>0</v>
+        <v>90</v>
+      </c>
+      <c r="I177" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J177" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K177" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L177" s="2">
+        <v>0</v>
+      </c>
+      <c r="M177" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N177" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O177" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P177" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="Q177">
         <v>0</v>
@@ -44927,17 +44978,17 @@
       <c r="R177">
         <v>0</v>
       </c>
-      <c r="S177">
-        <v>0</v>
-      </c>
-      <c r="T177">
-        <v>0</v>
-      </c>
-      <c r="U177">
-        <v>0</v>
-      </c>
-      <c r="V177">
-        <v>0</v>
+      <c r="S177" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T177" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U177" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V177" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="W177" s="2" t="s">
         <v>41</v>
@@ -44952,10 +45003,10 @@
         <v>0</v>
       </c>
       <c r="AA177">
-        <v>170</v>
+        <v>250</v>
       </c>
       <c r="AB177">
-        <v>170</v>
+        <v>90</v>
       </c>
       <c r="AC177">
         <v>0</v>
@@ -45117,6 +45168,1706 @@
         <v>0</v>
       </c>
       <c r="CD177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A178" s="4">
+        <v>175</v>
+      </c>
+      <c r="B178" s="5">
+        <v>46002</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D178" t="s">
+        <v>267</v>
+      </c>
+      <c r="F178" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="G178">
+        <v>250</v>
+      </c>
+      <c r="H178">
+        <v>90</v>
+      </c>
+      <c r="I178" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J178" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K178" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L178" s="2">
+        <v>0</v>
+      </c>
+      <c r="M178" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N178" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O178" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P178" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q178">
+        <v>0</v>
+      </c>
+      <c r="R178">
+        <v>0</v>
+      </c>
+      <c r="S178" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T178" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U178" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V178" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W178" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X178">
+        <v>0</v>
+      </c>
+      <c r="Y178" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z178" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA178">
+        <v>250</v>
+      </c>
+      <c r="AB178">
+        <v>90</v>
+      </c>
+      <c r="AC178">
+        <v>0</v>
+      </c>
+      <c r="AD178">
+        <v>0</v>
+      </c>
+      <c r="AE178">
+        <v>0</v>
+      </c>
+      <c r="AF178">
+        <v>0</v>
+      </c>
+      <c r="AG178">
+        <v>0</v>
+      </c>
+      <c r="AH178">
+        <v>0</v>
+      </c>
+      <c r="AI178">
+        <v>0</v>
+      </c>
+      <c r="AJ178">
+        <v>0</v>
+      </c>
+      <c r="AK178">
+        <v>0</v>
+      </c>
+      <c r="AL178">
+        <v>0</v>
+      </c>
+      <c r="AM178">
+        <v>0</v>
+      </c>
+      <c r="AN178">
+        <v>0</v>
+      </c>
+      <c r="AO178">
+        <v>0</v>
+      </c>
+      <c r="AP178">
+        <v>0</v>
+      </c>
+      <c r="AQ178" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR178">
+        <v>0</v>
+      </c>
+      <c r="AS178" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT178">
+        <v>0</v>
+      </c>
+      <c r="AU178">
+        <v>0</v>
+      </c>
+      <c r="AV178">
+        <v>0</v>
+      </c>
+      <c r="AW178">
+        <v>0</v>
+      </c>
+      <c r="AX178">
+        <v>0</v>
+      </c>
+      <c r="AY178">
+        <v>0</v>
+      </c>
+      <c r="AZ178">
+        <v>0</v>
+      </c>
+      <c r="BA178">
+        <v>0</v>
+      </c>
+      <c r="BB178">
+        <v>0</v>
+      </c>
+      <c r="BC178">
+        <v>0</v>
+      </c>
+      <c r="BD178">
+        <v>0</v>
+      </c>
+      <c r="BE178">
+        <v>0</v>
+      </c>
+      <c r="BF178">
+        <v>0</v>
+      </c>
+      <c r="BG178">
+        <v>0</v>
+      </c>
+      <c r="BH178">
+        <v>0</v>
+      </c>
+      <c r="BI178">
+        <v>0</v>
+      </c>
+      <c r="BJ178">
+        <v>0</v>
+      </c>
+      <c r="BK178" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL178">
+        <v>0</v>
+      </c>
+      <c r="BM178" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN178">
+        <v>0</v>
+      </c>
+      <c r="BO178">
+        <v>0</v>
+      </c>
+      <c r="BP178">
+        <v>0</v>
+      </c>
+      <c r="BQ178">
+        <v>0</v>
+      </c>
+      <c r="BR178">
+        <v>0</v>
+      </c>
+      <c r="BS178">
+        <v>0</v>
+      </c>
+      <c r="BT178">
+        <v>0</v>
+      </c>
+      <c r="BU178">
+        <v>0</v>
+      </c>
+      <c r="BV178">
+        <v>0</v>
+      </c>
+      <c r="BW178">
+        <v>0</v>
+      </c>
+      <c r="BX178">
+        <v>0</v>
+      </c>
+      <c r="BY178">
+        <v>0</v>
+      </c>
+      <c r="BZ178">
+        <v>0</v>
+      </c>
+      <c r="CA178">
+        <v>0</v>
+      </c>
+      <c r="CB178">
+        <v>0</v>
+      </c>
+      <c r="CC178">
+        <v>0</v>
+      </c>
+      <c r="CD178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A179" s="4">
+        <v>176</v>
+      </c>
+      <c r="B179" s="5">
+        <v>46002</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D179" t="s">
+        <v>263</v>
+      </c>
+      <c r="F179" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="G179">
+        <v>250</v>
+      </c>
+      <c r="H179">
+        <v>90</v>
+      </c>
+      <c r="I179" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J179" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K179" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L179" s="2">
+        <v>0</v>
+      </c>
+      <c r="M179" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N179" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O179" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P179" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q179">
+        <v>0</v>
+      </c>
+      <c r="R179">
+        <v>0</v>
+      </c>
+      <c r="S179" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T179" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U179" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V179" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="W179" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X179">
+        <v>0</v>
+      </c>
+      <c r="Y179" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z179" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA179">
+        <v>250</v>
+      </c>
+      <c r="AB179">
+        <v>90</v>
+      </c>
+      <c r="AC179">
+        <v>0</v>
+      </c>
+      <c r="AD179">
+        <v>0</v>
+      </c>
+      <c r="AE179">
+        <v>0</v>
+      </c>
+      <c r="AF179">
+        <v>0</v>
+      </c>
+      <c r="AG179">
+        <v>0</v>
+      </c>
+      <c r="AH179">
+        <v>0</v>
+      </c>
+      <c r="AI179">
+        <v>0</v>
+      </c>
+      <c r="AJ179">
+        <v>0</v>
+      </c>
+      <c r="AK179">
+        <v>0</v>
+      </c>
+      <c r="AL179">
+        <v>0</v>
+      </c>
+      <c r="AM179">
+        <v>0</v>
+      </c>
+      <c r="AN179">
+        <v>0</v>
+      </c>
+      <c r="AO179">
+        <v>0</v>
+      </c>
+      <c r="AP179">
+        <v>0</v>
+      </c>
+      <c r="AQ179" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR179">
+        <v>0</v>
+      </c>
+      <c r="AS179" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT179">
+        <v>0</v>
+      </c>
+      <c r="AU179">
+        <v>0</v>
+      </c>
+      <c r="AV179">
+        <v>0</v>
+      </c>
+      <c r="AW179">
+        <v>0</v>
+      </c>
+      <c r="AX179">
+        <v>0</v>
+      </c>
+      <c r="AY179">
+        <v>0</v>
+      </c>
+      <c r="AZ179">
+        <v>0</v>
+      </c>
+      <c r="BA179">
+        <v>0</v>
+      </c>
+      <c r="BB179">
+        <v>0</v>
+      </c>
+      <c r="BC179">
+        <v>0</v>
+      </c>
+      <c r="BD179">
+        <v>0</v>
+      </c>
+      <c r="BE179">
+        <v>0</v>
+      </c>
+      <c r="BF179">
+        <v>0</v>
+      </c>
+      <c r="BG179">
+        <v>0</v>
+      </c>
+      <c r="BH179">
+        <v>0</v>
+      </c>
+      <c r="BI179">
+        <v>0</v>
+      </c>
+      <c r="BJ179">
+        <v>0</v>
+      </c>
+      <c r="BK179" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL179">
+        <v>0</v>
+      </c>
+      <c r="BM179" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN179">
+        <v>0</v>
+      </c>
+      <c r="BO179">
+        <v>0</v>
+      </c>
+      <c r="BP179">
+        <v>0</v>
+      </c>
+      <c r="BQ179">
+        <v>0</v>
+      </c>
+      <c r="BR179">
+        <v>0</v>
+      </c>
+      <c r="BS179">
+        <v>0</v>
+      </c>
+      <c r="BT179">
+        <v>0</v>
+      </c>
+      <c r="BU179">
+        <v>0</v>
+      </c>
+      <c r="BV179">
+        <v>0</v>
+      </c>
+      <c r="BW179">
+        <v>0</v>
+      </c>
+      <c r="BX179">
+        <v>0</v>
+      </c>
+      <c r="BY179">
+        <v>0</v>
+      </c>
+      <c r="BZ179">
+        <v>0</v>
+      </c>
+      <c r="CA179">
+        <v>0</v>
+      </c>
+      <c r="CB179">
+        <v>0</v>
+      </c>
+      <c r="CC179">
+        <v>0</v>
+      </c>
+      <c r="CD179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A180" s="4">
+        <v>177</v>
+      </c>
+      <c r="B180" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F180" t="s">
+        <v>217</v>
+      </c>
+      <c r="G180">
+        <v>170</v>
+      </c>
+      <c r="H180">
+        <v>170</v>
+      </c>
+      <c r="I180" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J180" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K180" s="2">
+        <v>0</v>
+      </c>
+      <c r="L180" s="2">
+        <v>0</v>
+      </c>
+      <c r="M180" s="2">
+        <v>0</v>
+      </c>
+      <c r="N180" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O180" s="2">
+        <v>0</v>
+      </c>
+      <c r="P180" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q180" s="2">
+        <v>0</v>
+      </c>
+      <c r="R180" s="2">
+        <v>0</v>
+      </c>
+      <c r="S180" s="2">
+        <v>0</v>
+      </c>
+      <c r="T180" s="2">
+        <v>0</v>
+      </c>
+      <c r="U180" s="2">
+        <v>0</v>
+      </c>
+      <c r="V180" s="2">
+        <v>0</v>
+      </c>
+      <c r="W180" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X180">
+        <v>0</v>
+      </c>
+      <c r="Y180" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z180" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA180">
+        <v>170</v>
+      </c>
+      <c r="AB180">
+        <v>170</v>
+      </c>
+      <c r="AC180">
+        <v>0</v>
+      </c>
+      <c r="AD180">
+        <v>0</v>
+      </c>
+      <c r="AE180">
+        <v>0</v>
+      </c>
+      <c r="AF180">
+        <v>0</v>
+      </c>
+      <c r="AG180">
+        <v>0</v>
+      </c>
+      <c r="AH180">
+        <v>0</v>
+      </c>
+      <c r="AI180">
+        <v>0</v>
+      </c>
+      <c r="AJ180">
+        <v>0</v>
+      </c>
+      <c r="AK180">
+        <v>0</v>
+      </c>
+      <c r="AL180">
+        <v>0</v>
+      </c>
+      <c r="AM180">
+        <v>0</v>
+      </c>
+      <c r="AN180">
+        <v>0</v>
+      </c>
+      <c r="AO180">
+        <v>0</v>
+      </c>
+      <c r="AP180">
+        <v>0</v>
+      </c>
+      <c r="AQ180" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR180">
+        <v>0</v>
+      </c>
+      <c r="AS180" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT180">
+        <v>0</v>
+      </c>
+      <c r="AU180">
+        <v>0</v>
+      </c>
+      <c r="AV180">
+        <v>0</v>
+      </c>
+      <c r="AW180">
+        <v>0</v>
+      </c>
+      <c r="AX180">
+        <v>0</v>
+      </c>
+      <c r="AY180">
+        <v>0</v>
+      </c>
+      <c r="AZ180">
+        <v>0</v>
+      </c>
+      <c r="BA180">
+        <v>0</v>
+      </c>
+      <c r="BB180">
+        <v>0</v>
+      </c>
+      <c r="BC180">
+        <v>0</v>
+      </c>
+      <c r="BD180">
+        <v>0</v>
+      </c>
+      <c r="BE180">
+        <v>0</v>
+      </c>
+      <c r="BF180">
+        <v>0</v>
+      </c>
+      <c r="BG180">
+        <v>0</v>
+      </c>
+      <c r="BH180">
+        <v>0</v>
+      </c>
+      <c r="BI180">
+        <v>0</v>
+      </c>
+      <c r="BJ180">
+        <v>0</v>
+      </c>
+      <c r="BK180" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL180">
+        <v>0</v>
+      </c>
+      <c r="BM180" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN180">
+        <v>0</v>
+      </c>
+      <c r="BO180">
+        <v>0</v>
+      </c>
+      <c r="BP180">
+        <v>0</v>
+      </c>
+      <c r="BQ180">
+        <v>0</v>
+      </c>
+      <c r="BR180">
+        <v>0</v>
+      </c>
+      <c r="BS180">
+        <v>0</v>
+      </c>
+      <c r="BT180">
+        <v>0</v>
+      </c>
+      <c r="BU180">
+        <v>0</v>
+      </c>
+      <c r="BV180">
+        <v>0</v>
+      </c>
+      <c r="BW180">
+        <v>0</v>
+      </c>
+      <c r="BX180">
+        <v>0</v>
+      </c>
+      <c r="BY180">
+        <v>0</v>
+      </c>
+      <c r="BZ180">
+        <v>0</v>
+      </c>
+      <c r="CA180">
+        <v>0</v>
+      </c>
+      <c r="CB180">
+        <v>0</v>
+      </c>
+      <c r="CC180">
+        <v>0</v>
+      </c>
+      <c r="CD180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A181" s="4">
+        <v>178</v>
+      </c>
+      <c r="B181" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C181" t="s">
+        <v>214</v>
+      </c>
+      <c r="F181" t="s">
+        <v>217</v>
+      </c>
+      <c r="G181">
+        <v>170</v>
+      </c>
+      <c r="H181">
+        <v>170</v>
+      </c>
+      <c r="I181">
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+      <c r="M181">
+        <v>0</v>
+      </c>
+      <c r="N181">
+        <v>0</v>
+      </c>
+      <c r="O181">
+        <v>0</v>
+      </c>
+      <c r="P181">
+        <v>0</v>
+      </c>
+      <c r="Q181">
+        <v>0</v>
+      </c>
+      <c r="R181">
+        <v>0</v>
+      </c>
+      <c r="S181">
+        <v>0</v>
+      </c>
+      <c r="T181">
+        <v>0</v>
+      </c>
+      <c r="U181">
+        <v>0</v>
+      </c>
+      <c r="V181">
+        <v>0</v>
+      </c>
+      <c r="W181" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X181">
+        <v>0</v>
+      </c>
+      <c r="Y181" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z181" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA181">
+        <v>170</v>
+      </c>
+      <c r="AB181">
+        <v>170</v>
+      </c>
+      <c r="AC181">
+        <v>0</v>
+      </c>
+      <c r="AD181">
+        <v>0</v>
+      </c>
+      <c r="AE181">
+        <v>0</v>
+      </c>
+      <c r="AF181">
+        <v>0</v>
+      </c>
+      <c r="AG181">
+        <v>0</v>
+      </c>
+      <c r="AH181">
+        <v>0</v>
+      </c>
+      <c r="AI181">
+        <v>0</v>
+      </c>
+      <c r="AJ181">
+        <v>0</v>
+      </c>
+      <c r="AK181">
+        <v>0</v>
+      </c>
+      <c r="AL181">
+        <v>0</v>
+      </c>
+      <c r="AM181">
+        <v>0</v>
+      </c>
+      <c r="AN181">
+        <v>0</v>
+      </c>
+      <c r="AO181">
+        <v>0</v>
+      </c>
+      <c r="AP181">
+        <v>0</v>
+      </c>
+      <c r="AQ181" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR181">
+        <v>0</v>
+      </c>
+      <c r="AS181" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT181">
+        <v>0</v>
+      </c>
+      <c r="AU181">
+        <v>0</v>
+      </c>
+      <c r="AV181">
+        <v>0</v>
+      </c>
+      <c r="AW181">
+        <v>0</v>
+      </c>
+      <c r="AX181">
+        <v>0</v>
+      </c>
+      <c r="AY181">
+        <v>0</v>
+      </c>
+      <c r="AZ181">
+        <v>0</v>
+      </c>
+      <c r="BA181">
+        <v>0</v>
+      </c>
+      <c r="BB181">
+        <v>0</v>
+      </c>
+      <c r="BC181">
+        <v>0</v>
+      </c>
+      <c r="BD181">
+        <v>0</v>
+      </c>
+      <c r="BE181">
+        <v>0</v>
+      </c>
+      <c r="BF181">
+        <v>0</v>
+      </c>
+      <c r="BG181">
+        <v>0</v>
+      </c>
+      <c r="BH181">
+        <v>0</v>
+      </c>
+      <c r="BI181">
+        <v>0</v>
+      </c>
+      <c r="BJ181">
+        <v>0</v>
+      </c>
+      <c r="BK181" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL181">
+        <v>0</v>
+      </c>
+      <c r="BM181" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN181">
+        <v>0</v>
+      </c>
+      <c r="BO181">
+        <v>0</v>
+      </c>
+      <c r="BP181">
+        <v>0</v>
+      </c>
+      <c r="BQ181">
+        <v>0</v>
+      </c>
+      <c r="BR181">
+        <v>0</v>
+      </c>
+      <c r="BS181">
+        <v>0</v>
+      </c>
+      <c r="BT181">
+        <v>0</v>
+      </c>
+      <c r="BU181">
+        <v>0</v>
+      </c>
+      <c r="BV181">
+        <v>0</v>
+      </c>
+      <c r="BW181">
+        <v>0</v>
+      </c>
+      <c r="BX181">
+        <v>0</v>
+      </c>
+      <c r="BY181">
+        <v>0</v>
+      </c>
+      <c r="BZ181">
+        <v>0</v>
+      </c>
+      <c r="CA181">
+        <v>0</v>
+      </c>
+      <c r="CB181">
+        <v>0</v>
+      </c>
+      <c r="CC181">
+        <v>0</v>
+      </c>
+      <c r="CD181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A182" s="4">
+        <v>179</v>
+      </c>
+      <c r="B182" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C182" t="s">
+        <v>215</v>
+      </c>
+      <c r="F182" t="s">
+        <v>217</v>
+      </c>
+      <c r="G182">
+        <v>170</v>
+      </c>
+      <c r="H182">
+        <v>170</v>
+      </c>
+      <c r="I182">
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+      <c r="K182">
+        <v>0</v>
+      </c>
+      <c r="L182">
+        <v>0</v>
+      </c>
+      <c r="M182">
+        <v>0</v>
+      </c>
+      <c r="N182">
+        <v>0</v>
+      </c>
+      <c r="O182">
+        <v>0</v>
+      </c>
+      <c r="P182">
+        <v>0</v>
+      </c>
+      <c r="Q182">
+        <v>0</v>
+      </c>
+      <c r="R182">
+        <v>0</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+      <c r="T182">
+        <v>0</v>
+      </c>
+      <c r="U182">
+        <v>0</v>
+      </c>
+      <c r="V182">
+        <v>0</v>
+      </c>
+      <c r="W182" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X182">
+        <v>0</v>
+      </c>
+      <c r="Y182" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z182" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA182">
+        <v>170</v>
+      </c>
+      <c r="AB182">
+        <v>170</v>
+      </c>
+      <c r="AC182">
+        <v>0</v>
+      </c>
+      <c r="AD182">
+        <v>0</v>
+      </c>
+      <c r="AE182">
+        <v>0</v>
+      </c>
+      <c r="AF182">
+        <v>0</v>
+      </c>
+      <c r="AG182">
+        <v>0</v>
+      </c>
+      <c r="AH182">
+        <v>0</v>
+      </c>
+      <c r="AI182">
+        <v>0</v>
+      </c>
+      <c r="AJ182">
+        <v>0</v>
+      </c>
+      <c r="AK182">
+        <v>0</v>
+      </c>
+      <c r="AL182">
+        <v>0</v>
+      </c>
+      <c r="AM182">
+        <v>0</v>
+      </c>
+      <c r="AN182">
+        <v>0</v>
+      </c>
+      <c r="AO182">
+        <v>0</v>
+      </c>
+      <c r="AP182">
+        <v>0</v>
+      </c>
+      <c r="AQ182" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR182">
+        <v>0</v>
+      </c>
+      <c r="AS182" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT182">
+        <v>0</v>
+      </c>
+      <c r="AU182">
+        <v>0</v>
+      </c>
+      <c r="AV182">
+        <v>0</v>
+      </c>
+      <c r="AW182">
+        <v>0</v>
+      </c>
+      <c r="AX182">
+        <v>0</v>
+      </c>
+      <c r="AY182">
+        <v>0</v>
+      </c>
+      <c r="AZ182">
+        <v>0</v>
+      </c>
+      <c r="BA182">
+        <v>0</v>
+      </c>
+      <c r="BB182">
+        <v>0</v>
+      </c>
+      <c r="BC182">
+        <v>0</v>
+      </c>
+      <c r="BD182">
+        <v>0</v>
+      </c>
+      <c r="BE182">
+        <v>0</v>
+      </c>
+      <c r="BF182">
+        <v>0</v>
+      </c>
+      <c r="BG182">
+        <v>0</v>
+      </c>
+      <c r="BH182">
+        <v>0</v>
+      </c>
+      <c r="BI182">
+        <v>0</v>
+      </c>
+      <c r="BJ182">
+        <v>0</v>
+      </c>
+      <c r="BK182" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL182">
+        <v>0</v>
+      </c>
+      <c r="BM182" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN182">
+        <v>0</v>
+      </c>
+      <c r="BO182">
+        <v>0</v>
+      </c>
+      <c r="BP182">
+        <v>0</v>
+      </c>
+      <c r="BQ182">
+        <v>0</v>
+      </c>
+      <c r="BR182">
+        <v>0</v>
+      </c>
+      <c r="BS182">
+        <v>0</v>
+      </c>
+      <c r="BT182">
+        <v>0</v>
+      </c>
+      <c r="BU182">
+        <v>0</v>
+      </c>
+      <c r="BV182">
+        <v>0</v>
+      </c>
+      <c r="BW182">
+        <v>0</v>
+      </c>
+      <c r="BX182">
+        <v>0</v>
+      </c>
+      <c r="BY182">
+        <v>0</v>
+      </c>
+      <c r="BZ182">
+        <v>0</v>
+      </c>
+      <c r="CA182">
+        <v>0</v>
+      </c>
+      <c r="CB182">
+        <v>0</v>
+      </c>
+      <c r="CC182">
+        <v>0</v>
+      </c>
+      <c r="CD182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A183" s="4">
+        <v>180</v>
+      </c>
+      <c r="B183" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C183">
+        <v>404</v>
+      </c>
+      <c r="F183" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="G183">
+        <v>240</v>
+      </c>
+      <c r="H183">
+        <v>180</v>
+      </c>
+      <c r="I183">
+        <v>0</v>
+      </c>
+      <c r="J183">
+        <v>0</v>
+      </c>
+      <c r="K183">
+        <v>0</v>
+      </c>
+      <c r="L183">
+        <v>0</v>
+      </c>
+      <c r="M183">
+        <v>0</v>
+      </c>
+      <c r="N183">
+        <v>0</v>
+      </c>
+      <c r="O183">
+        <v>0</v>
+      </c>
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="Q183">
+        <v>0</v>
+      </c>
+      <c r="R183">
+        <v>0</v>
+      </c>
+      <c r="S183">
+        <v>0</v>
+      </c>
+      <c r="T183">
+        <v>0</v>
+      </c>
+      <c r="U183">
+        <v>0</v>
+      </c>
+      <c r="V183">
+        <v>0</v>
+      </c>
+      <c r="W183" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X183">
+        <v>0</v>
+      </c>
+      <c r="Y183" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z183" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA183">
+        <v>170</v>
+      </c>
+      <c r="AB183">
+        <v>170</v>
+      </c>
+      <c r="AC183">
+        <v>0</v>
+      </c>
+      <c r="AD183">
+        <v>0</v>
+      </c>
+      <c r="AE183">
+        <v>0</v>
+      </c>
+      <c r="AF183">
+        <v>0</v>
+      </c>
+      <c r="AG183">
+        <v>0</v>
+      </c>
+      <c r="AH183">
+        <v>0</v>
+      </c>
+      <c r="AI183">
+        <v>0</v>
+      </c>
+      <c r="AJ183">
+        <v>0</v>
+      </c>
+      <c r="AK183">
+        <v>0</v>
+      </c>
+      <c r="AL183">
+        <v>0</v>
+      </c>
+      <c r="AM183">
+        <v>0</v>
+      </c>
+      <c r="AN183">
+        <v>0</v>
+      </c>
+      <c r="AO183">
+        <v>0</v>
+      </c>
+      <c r="AP183">
+        <v>0</v>
+      </c>
+      <c r="AQ183" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR183">
+        <v>0</v>
+      </c>
+      <c r="AS183" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT183">
+        <v>0</v>
+      </c>
+      <c r="AU183">
+        <v>0</v>
+      </c>
+      <c r="AV183">
+        <v>0</v>
+      </c>
+      <c r="AW183">
+        <v>0</v>
+      </c>
+      <c r="AX183">
+        <v>0</v>
+      </c>
+      <c r="AY183">
+        <v>0</v>
+      </c>
+      <c r="AZ183">
+        <v>0</v>
+      </c>
+      <c r="BA183">
+        <v>0</v>
+      </c>
+      <c r="BB183">
+        <v>0</v>
+      </c>
+      <c r="BC183">
+        <v>0</v>
+      </c>
+      <c r="BD183">
+        <v>0</v>
+      </c>
+      <c r="BE183">
+        <v>0</v>
+      </c>
+      <c r="BF183">
+        <v>0</v>
+      </c>
+      <c r="BG183">
+        <v>0</v>
+      </c>
+      <c r="BH183">
+        <v>0</v>
+      </c>
+      <c r="BI183">
+        <v>0</v>
+      </c>
+      <c r="BJ183">
+        <v>0</v>
+      </c>
+      <c r="BK183" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL183">
+        <v>0</v>
+      </c>
+      <c r="BM183" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN183">
+        <v>0</v>
+      </c>
+      <c r="BO183">
+        <v>0</v>
+      </c>
+      <c r="BP183">
+        <v>0</v>
+      </c>
+      <c r="BQ183">
+        <v>0</v>
+      </c>
+      <c r="BR183">
+        <v>0</v>
+      </c>
+      <c r="BS183">
+        <v>0</v>
+      </c>
+      <c r="BT183">
+        <v>0</v>
+      </c>
+      <c r="BU183">
+        <v>0</v>
+      </c>
+      <c r="BV183">
+        <v>0</v>
+      </c>
+      <c r="BW183">
+        <v>0</v>
+      </c>
+      <c r="BX183">
+        <v>0</v>
+      </c>
+      <c r="BY183">
+        <v>0</v>
+      </c>
+      <c r="BZ183">
+        <v>0</v>
+      </c>
+      <c r="CA183">
+        <v>0</v>
+      </c>
+      <c r="CB183">
+        <v>0</v>
+      </c>
+      <c r="CC183">
+        <v>0</v>
+      </c>
+      <c r="CD183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:82" x14ac:dyDescent="0.2">
+      <c r="A184" s="4">
+        <v>404</v>
+      </c>
+      <c r="B184" s="5">
+        <v>45693</v>
+      </c>
+      <c r="C184">
+        <v>404</v>
+      </c>
+      <c r="F184" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="G184">
+        <v>240</v>
+      </c>
+      <c r="H184">
+        <v>180</v>
+      </c>
+      <c r="I184">
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>0</v>
+      </c>
+      <c r="L184">
+        <v>0</v>
+      </c>
+      <c r="M184">
+        <v>0</v>
+      </c>
+      <c r="N184">
+        <v>0</v>
+      </c>
+      <c r="O184">
+        <v>0</v>
+      </c>
+      <c r="P184">
+        <v>0</v>
+      </c>
+      <c r="Q184">
+        <v>0</v>
+      </c>
+      <c r="R184">
+        <v>0</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+      <c r="T184">
+        <v>0</v>
+      </c>
+      <c r="U184">
+        <v>0</v>
+      </c>
+      <c r="V184">
+        <v>0</v>
+      </c>
+      <c r="W184" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="X184">
+        <v>0</v>
+      </c>
+      <c r="Y184" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z184" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA184">
+        <v>170</v>
+      </c>
+      <c r="AB184">
+        <v>170</v>
+      </c>
+      <c r="AC184">
+        <v>0</v>
+      </c>
+      <c r="AD184">
+        <v>0</v>
+      </c>
+      <c r="AE184">
+        <v>0</v>
+      </c>
+      <c r="AF184">
+        <v>0</v>
+      </c>
+      <c r="AG184">
+        <v>0</v>
+      </c>
+      <c r="AH184">
+        <v>0</v>
+      </c>
+      <c r="AI184">
+        <v>0</v>
+      </c>
+      <c r="AJ184">
+        <v>0</v>
+      </c>
+      <c r="AK184">
+        <v>0</v>
+      </c>
+      <c r="AL184">
+        <v>0</v>
+      </c>
+      <c r="AM184">
+        <v>0</v>
+      </c>
+      <c r="AN184">
+        <v>0</v>
+      </c>
+      <c r="AO184">
+        <v>0</v>
+      </c>
+      <c r="AP184">
+        <v>0</v>
+      </c>
+      <c r="AQ184" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR184">
+        <v>0</v>
+      </c>
+      <c r="AS184" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="AT184">
+        <v>0</v>
+      </c>
+      <c r="AU184">
+        <v>0</v>
+      </c>
+      <c r="AV184">
+        <v>0</v>
+      </c>
+      <c r="AW184">
+        <v>0</v>
+      </c>
+      <c r="AX184">
+        <v>0</v>
+      </c>
+      <c r="AY184">
+        <v>0</v>
+      </c>
+      <c r="AZ184">
+        <v>0</v>
+      </c>
+      <c r="BA184">
+        <v>0</v>
+      </c>
+      <c r="BB184">
+        <v>0</v>
+      </c>
+      <c r="BC184">
+        <v>0</v>
+      </c>
+      <c r="BD184">
+        <v>0</v>
+      </c>
+      <c r="BE184">
+        <v>0</v>
+      </c>
+      <c r="BF184">
+        <v>0</v>
+      </c>
+      <c r="BG184">
+        <v>0</v>
+      </c>
+      <c r="BH184">
+        <v>0</v>
+      </c>
+      <c r="BI184">
+        <v>0</v>
+      </c>
+      <c r="BJ184">
+        <v>0</v>
+      </c>
+      <c r="BK184" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="BL184">
+        <v>0</v>
+      </c>
+      <c r="BM184" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="BN184">
+        <v>0</v>
+      </c>
+      <c r="BO184">
+        <v>0</v>
+      </c>
+      <c r="BP184">
+        <v>0</v>
+      </c>
+      <c r="BQ184">
+        <v>0</v>
+      </c>
+      <c r="BR184">
+        <v>0</v>
+      </c>
+      <c r="BS184">
+        <v>0</v>
+      </c>
+      <c r="BT184">
+        <v>0</v>
+      </c>
+      <c r="BU184">
+        <v>0</v>
+      </c>
+      <c r="BV184">
+        <v>0</v>
+      </c>
+      <c r="BW184">
+        <v>0</v>
+      </c>
+      <c r="BX184">
+        <v>0</v>
+      </c>
+      <c r="BY184">
+        <v>0</v>
+      </c>
+      <c r="BZ184">
+        <v>0</v>
+      </c>
+      <c r="CA184">
+        <v>0</v>
+      </c>
+      <c r="CB184">
+        <v>0</v>
+      </c>
+      <c r="CC184">
+        <v>0</v>
+      </c>
+      <c r="CD184">
         <v>0</v>
       </c>
     </row>
@@ -45133,11 +46884,21 @@
     <hyperlink ref="F138" r:id="rId8" xr:uid="{C4BFBD49-530E-449E-B29C-6619C4A43276}"/>
     <hyperlink ref="F4" r:id="rId9" xr:uid="{16353D1E-1B5D-470D-B307-8D2218647691}"/>
     <hyperlink ref="F166" r:id="rId10" xr:uid="{B2839A20-3FC5-49C4-A010-C20261BE5986}"/>
-    <hyperlink ref="F176" r:id="rId11" xr:uid="{B0B01E66-2991-40C6-9A40-7D161D71D2A9}"/>
+    <hyperlink ref="F183" r:id="rId11" xr:uid="{B0B01E66-2991-40C6-9A40-7D161D71D2A9}"/>
     <hyperlink ref="F58" r:id="rId12" xr:uid="{366D18FC-0AC7-4944-8D7D-3BE1139D289A}"/>
-    <hyperlink ref="F177" r:id="rId13" xr:uid="{5D884C4A-B40B-4330-840A-58B5792571E4}"/>
+    <hyperlink ref="F184" r:id="rId13" xr:uid="{5D884C4A-B40B-4330-840A-58B5792571E4}"/>
+    <hyperlink ref="F170" r:id="rId14" xr:uid="{ACDFEFB3-652A-4D78-B1C4-9ABEFC4BA93C}"/>
+    <hyperlink ref="F172" r:id="rId15" xr:uid="{318BCBB9-4822-491F-96DB-02B06E243D61}"/>
+    <hyperlink ref="F175" r:id="rId16" xr:uid="{FF9256DD-75C1-4AF6-BFAD-6E038D7CF6C0}"/>
+    <hyperlink ref="F173" r:id="rId17" xr:uid="{69620E1E-005D-4A4B-9081-4987C25675F1}"/>
+    <hyperlink ref="F171" r:id="rId18" xr:uid="{B8D0DA4C-7F7F-4AE1-BBF5-C4CAEED575F4}"/>
+    <hyperlink ref="F174" r:id="rId19" xr:uid="{5162792B-9B22-4940-B5E7-9540B9A25917}"/>
+    <hyperlink ref="F177" r:id="rId20" xr:uid="{A86B32FB-EA75-4FCA-A104-F2439F72FEA1}"/>
+    <hyperlink ref="F178" r:id="rId21" xr:uid="{D993F43D-F0E6-40B5-A1D7-BA94B71BF6D6}"/>
+    <hyperlink ref="F179" r:id="rId22" xr:uid="{00F68D3D-28AB-4513-8214-83EE213CF9EB}"/>
+    <hyperlink ref="F176" r:id="rId23" xr:uid="{30C78982-FCC1-4F74-B54D-6127496F5209}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId14"/>
+  <pageSetup paperSize="9" scale="57" fitToHeight="0" orientation="landscape" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>